<commit_message>
Point all dashboards to Data Source folder on Desktop
CRITICAL FIX:
- All dashboards now read DIRECTLY from Data Source folder
- No more copying files to project data folder
- Always uses latest data from Desktop/Operations Hub/Data Source/

File Paths Updated:
✅ CRM: ~/Desktop/Operations Hub/Data Source/CRM Data.xlsx
✅ ARC: ~/Desktop/Operations Hub/Data Source/ARC Configurations.xlsx
✅ Integration: ~/Desktop/Operations Hub/Data Source/Integration Access Board.xlsx
✅ Regression: ~/Desktop/Operations Hub/Data Source/E2E Testing Check .xlsx

Test Results:
✅ CRM: 159 records loaded
✅ ARC: 245 records loaded
✅ Integration: 268 records loaded (all 5 sheets)
✅ Regression: 313 records loaded

Benefits:
- No manual file copying needed
- Always reads latest data
- Single source of truth (Data Source folder)
- Easier to update data (just save to Data Source folder)
</commit_message>
<xml_diff>
--- a/data/Integration Access Board.xlsx
+++ b/data/Integration Access Board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tekion-my.sharepoint.com/personal/jyothik_tekion_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF136479-2486-450B-8F67-8A3DDE38451D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ACFFC5F-7429-4B6A-9164-7095A18A6D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{997D09BE-9057-5840-9899-6298661F320E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{997D09BE-9057-5840-9899-6298661F320E}"/>
   </bookViews>
   <sheets>
     <sheet name="August Go Live" sheetId="1" r:id="rId1"/>
@@ -1177,7 +1177,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="167" formatCode="[$-809]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1466,7 +1466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1583,12 +1583,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1607,12 +1601,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1625,9 +1613,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1693,6 +1678,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2044,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D9CE80-E408-CE41-A24B-779A9E8CDB9F}">
   <dimension ref="A1:BD250"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView showGridLines="0" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -2365,10 +2359,10 @@
       <c r="X5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="BB5" s="63" t="s">
+      <c r="BB5" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="BC5" s="63" t="s">
+      <c r="BC5" s="58" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2433,10 +2427,10 @@
       <c r="X6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="BB6" s="64" t="s">
+      <c r="BB6" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="BC6" s="65" t="s">
+      <c r="BC6" s="60" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2501,10 +2495,10 @@
       <c r="X7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="BB7" s="64" t="s">
+      <c r="BB7" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="BC7" s="65" t="s">
+      <c r="BC7" s="60" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2563,10 +2557,10 @@
       <c r="R8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BB8" s="64" t="s">
+      <c r="BB8" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="BC8" s="65" t="s">
+      <c r="BC8" s="60" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2627,10 +2621,10 @@
       <c r="R9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BB9" s="64" t="s">
+      <c r="BB9" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="BC9" s="65" t="s">
+      <c r="BC9" s="60" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2689,10 +2683,10 @@
         <v>18</v>
       </c>
       <c r="R10" s="2"/>
-      <c r="BB10" s="64" t="s">
+      <c r="BB10" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="BC10" s="65" t="s">
+      <c r="BC10" s="60" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2753,10 +2747,10 @@
       <c r="R11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BB11" s="64" t="s">
+      <c r="BB11" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="BC11" s="65" t="s">
+      <c r="BC11" s="60" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2817,10 +2811,10 @@
       <c r="R12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BB12" s="64" t="s">
+      <c r="BB12" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="BC12" s="65" t="s">
+      <c r="BC12" s="60" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2881,10 +2875,10 @@
       <c r="R13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BB13" s="64" t="s">
+      <c r="BB13" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="BC13" s="65" t="s">
+      <c r="BC13" s="60" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2945,10 +2939,10 @@
       <c r="R14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BB14" s="64" t="s">
+      <c r="BB14" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="BC14" s="65" t="s">
+      <c r="BC14" s="60" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3009,10 +3003,10 @@
       <c r="R15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BB15" s="64" t="s">
+      <c r="BB15" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="BC15" s="65" t="s">
+      <c r="BC15" s="60" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3073,10 +3067,10 @@
       <c r="R16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BB16" s="64" t="s">
+      <c r="BB16" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="BC16" s="65" t="s">
+      <c r="BC16" s="60" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3137,10 +3131,10 @@
       <c r="R17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BB17" s="64" t="s">
+      <c r="BB17" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="BC17" s="66" t="s">
+      <c r="BC17" s="61" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3201,10 +3195,10 @@
       <c r="R18" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="BB18" s="65" t="s">
+      <c r="BB18" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="BC18" s="65" t="s">
+      <c r="BC18" s="60" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3265,10 +3259,10 @@
       <c r="R19" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BB19" s="65" t="s">
+      <c r="BB19" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="BC19" s="65" t="s">
+      <c r="BC19" s="60" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3317,10 +3311,10 @@
       <c r="R20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="BB20" s="65" t="s">
+      <c r="BB20" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="BC20" s="65" t="s">
+      <c r="BC20" s="60" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3381,10 +3375,10 @@
       <c r="R21" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="BB21" s="65" t="s">
+      <c r="BB21" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="BC21" s="65" t="s">
+      <c r="BC21" s="60" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3445,10 +3439,10 @@
       <c r="R22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BB22" s="65" t="s">
+      <c r="BB22" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="BC22" s="65" t="s">
+      <c r="BC22" s="60" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5444,10 +5438,10 @@
       <c r="F59" s="19"/>
       <c r="G59" s="19"/>
       <c r="R59" s="19"/>
-      <c r="BA59" s="61"/>
+      <c r="BA59" s="56"/>
       <c r="BB59"/>
       <c r="BC59"/>
-      <c r="BD59" s="62"/>
+      <c r="BD59" s="57"/>
     </row>
     <row r="60" spans="1:56" ht="15.75">
       <c r="D60" s="7"/>
@@ -5655,7 +5649,7 @@
   <dimension ref="A1:U68"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
@@ -7234,7 +7228,7 @@
       <c r="N31" s="3">
         <v>6</v>
       </c>
-      <c r="O31" s="58" t="s">
+      <c r="O31" s="54" t="s">
         <v>167</v>
       </c>
     </row>
@@ -7630,7 +7624,7 @@
       <c r="N39" s="3">
         <v>6</v>
       </c>
-      <c r="O39" s="58" t="s">
+      <c r="O39" s="54" t="s">
         <v>179</v>
       </c>
     </row>
@@ -7833,7 +7827,7 @@
       <c r="O43" s="3"/>
     </row>
     <row r="44" spans="1:15">
-      <c r="A44" s="67" t="s">
+      <c r="A44" s="62" t="s">
         <v>186</v>
       </c>
       <c r="B44" s="3">
@@ -7883,7 +7877,7 @@
       </c>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="67" t="s">
+      <c r="A45" s="62" t="s">
         <v>187</v>
       </c>
       <c r="B45" s="3">
@@ -7933,7 +7927,7 @@
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="67" t="s">
+      <c r="A46" s="62" t="s">
         <v>188</v>
       </c>
       <c r="B46" s="3">
@@ -7983,7 +7977,7 @@
       </c>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="67" t="s">
+      <c r="A47" s="62" t="s">
         <v>189</v>
       </c>
       <c r="B47" s="3">
@@ -8087,7 +8081,7 @@
       <c r="B49" s="18">
         <v>7062</v>
       </c>
-      <c r="C49" s="49">
+      <c r="C49" s="47">
         <v>45923</v>
       </c>
       <c r="D49" s="18" t="str">
@@ -8134,10 +8128,10 @@
       <c r="A50" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="B50" s="48">
+      <c r="B50" s="46">
         <v>7061</v>
       </c>
-      <c r="C50" s="49">
+      <c r="C50" s="47">
         <v>45923</v>
       </c>
       <c r="D50" s="18" t="str">
@@ -8184,10 +8178,10 @@
       <c r="A51" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="B51" s="48">
+      <c r="B51" s="46">
         <v>7083</v>
       </c>
-      <c r="C51" s="49">
+      <c r="C51" s="47">
         <v>45929</v>
       </c>
       <c r="D51" s="18" t="str">
@@ -8228,10 +8222,10 @@
       <c r="A52" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="B52" s="48">
+      <c r="B52" s="46">
         <v>7055</v>
       </c>
-      <c r="C52" s="49">
+      <c r="C52" s="47">
         <v>45929</v>
       </c>
       <c r="D52" s="18" t="str">
@@ -8272,7 +8266,7 @@
       <c r="B53" s="18">
         <v>6890</v>
       </c>
-      <c r="C53" s="49">
+      <c r="C53" s="47">
         <v>45930</v>
       </c>
       <c r="D53" s="18" t="str">
@@ -8316,7 +8310,7 @@
       <c r="B54" s="18">
         <v>6882</v>
       </c>
-      <c r="C54" s="49">
+      <c r="C54" s="47">
         <v>45930</v>
       </c>
       <c r="D54" s="18" t="str">
@@ -8360,7 +8354,7 @@
       <c r="B55" s="18">
         <v>5946</v>
       </c>
-      <c r="C55" s="49">
+      <c r="C55" s="47">
         <v>45930</v>
       </c>
       <c r="D55" s="18" t="str">
@@ -8406,7 +8400,7 @@
       <c r="B56" s="18">
         <v>5949</v>
       </c>
-      <c r="C56" s="49">
+      <c r="C56" s="47">
         <v>45930</v>
       </c>
       <c r="D56" s="18" t="str">
@@ -8450,7 +8444,7 @@
       <c r="B57" s="18">
         <v>5940</v>
       </c>
-      <c r="C57" s="49">
+      <c r="C57" s="47">
         <v>45930</v>
       </c>
       <c r="D57" s="18" t="str">
@@ -8494,7 +8488,7 @@
       <c r="B58" s="18">
         <v>5937</v>
       </c>
-      <c r="C58" s="49">
+      <c r="C58" s="47">
         <v>45930</v>
       </c>
       <c r="D58" s="18" t="str">
@@ -8538,7 +8532,7 @@
       <c r="B59" s="18">
         <v>5948</v>
       </c>
-      <c r="C59" s="49">
+      <c r="C59" s="47">
         <v>45930</v>
       </c>
       <c r="D59" s="18" t="str">
@@ -8584,7 +8578,7 @@
       <c r="B60" s="18">
         <v>5950</v>
       </c>
-      <c r="C60" s="49">
+      <c r="C60" s="47">
         <v>45930</v>
       </c>
       <c r="D60" s="18" t="str">
@@ -8628,7 +8622,7 @@
       <c r="B61" s="18">
         <v>5938</v>
       </c>
-      <c r="C61" s="49">
+      <c r="C61" s="47">
         <v>45930</v>
       </c>
       <c r="D61" s="18" t="str">
@@ -8672,7 +8666,7 @@
       <c r="B62" s="18">
         <v>5936</v>
       </c>
-      <c r="C62" s="49">
+      <c r="C62" s="47">
         <v>45930</v>
       </c>
       <c r="D62" s="18" t="str">
@@ -8716,7 +8710,7 @@
       <c r="B63" s="18">
         <v>5945</v>
       </c>
-      <c r="C63" s="49">
+      <c r="C63" s="47">
         <v>45930</v>
       </c>
       <c r="D63" s="18" t="str">
@@ -8762,7 +8756,7 @@
       <c r="B64" s="18">
         <v>5944</v>
       </c>
-      <c r="C64" s="49">
+      <c r="C64" s="47">
         <v>45930</v>
       </c>
       <c r="D64" s="18" t="str">
@@ -8806,7 +8800,7 @@
       <c r="B65" s="18">
         <v>5942</v>
       </c>
-      <c r="C65" s="49">
+      <c r="C65" s="47">
         <v>45930</v>
       </c>
       <c r="D65" s="18" t="str">
@@ -8850,7 +8844,7 @@
       <c r="B66" s="18">
         <v>7018</v>
       </c>
-      <c r="C66" s="49">
+      <c r="C66" s="47">
         <v>45930</v>
       </c>
       <c r="D66" s="18" t="str">
@@ -8893,10 +8887,10 @@
       <c r="A67" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="B67" s="48">
+      <c r="B67" s="46">
         <v>7063</v>
       </c>
-      <c r="C67" s="49">
+      <c r="C67" s="47">
         <v>45930</v>
       </c>
       <c r="D67" s="18" t="str">
@@ -8927,13 +8921,13 @@
       </c>
     </row>
     <row r="68" spans="1:15" s="17" customFormat="1">
-      <c r="A68" s="46" t="s">
+      <c r="A68" s="44" t="s">
         <v>213</v>
       </c>
       <c r="B68" s="18">
         <v>6879</v>
       </c>
-      <c r="C68" s="49">
+      <c r="C68" s="47">
         <v>45930</v>
       </c>
       <c r="D68" s="18" t="str">
@@ -8981,14 +8975,14 @@
   <dimension ref="A1:AB59"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="36.125" style="37" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.625" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.25" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="34" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.625" style="34" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.25" style="34" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.25" style="34" customWidth="1"/>
@@ -9060,27 +9054,27 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="70" customFormat="1">
-      <c r="A2" s="75" t="s">
+    <row r="2" spans="1:28" s="65" customFormat="1">
+      <c r="A2" s="70" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="44">
         <v>7084</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="80">
         <v>45931</v>
       </c>
       <c r="D2" s="18" t="str">
         <f ca="1">IF(C2-TODAY()&lt;0,"NA",C2-TODAY())</f>
         <v>NA</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="E2" s="70" t="s">
         <v>74</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="44" t="s">
         <v>38</v>
       </c>
       <c r="H2" s="20" t="s">
@@ -9090,71 +9084,71 @@
         <f>VLOOKUP(H2,$AA$1:$AB$9,2,0)</f>
         <v>Alex Rust</v>
       </c>
-      <c r="J2" s="75" t="s">
+      <c r="J2" s="70" t="s">
         <v>215</v>
       </c>
-      <c r="K2" s="75" t="s">
+      <c r="K2" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="68"/>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="72"/>
-    </row>
-    <row r="3" spans="1:28" s="70" customFormat="1">
-      <c r="A3" s="46" t="s">
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="63"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="67"/>
+    </row>
+    <row r="3" spans="1:28" s="65" customFormat="1">
+      <c r="A3" s="44" t="s">
         <v>216</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="44">
         <v>6982</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="81">
         <v>45937</v>
       </c>
       <c r="D3" s="18">
         <f ca="1">IF(C3-TODAY()&lt;0,"NA",C3-TODAY())</f>
         <v>0</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="44" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="18" t="str">
         <f>VLOOKUP(E3,'September Go Live'!E:F,2,0)</f>
         <v>Hanna Schneider</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="44" t="s">
         <v>33</v>
       </c>
       <c r="I3" s="18" t="str">
         <f>VLOOKUP(H3,$AA$1:$AB$9,2,0)</f>
         <v>Saurabh Tyagi</v>
       </c>
-      <c r="J3" s="73" t="s">
+      <c r="J3" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="73" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="68"/>
-      <c r="AA3" s="71"/>
-      <c r="AB3" s="72"/>
-    </row>
-    <row r="4" spans="1:28" s="70" customFormat="1">
+      <c r="K3" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="63"/>
+      <c r="AA3" s="66"/>
+      <c r="AB3" s="67"/>
+    </row>
+    <row r="4" spans="1:28" s="65" customFormat="1">
       <c r="A4" s="18" t="s">
         <v>217</v>
       </c>
       <c r="B4" s="20">
         <v>6931</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="81">
         <v>45931</v>
       </c>
       <c r="D4" s="18" t="str">
@@ -9202,14 +9196,14 @@
       <c r="AA4" s="34"/>
       <c r="AB4" s="34"/>
     </row>
-    <row r="5" spans="1:28" s="70" customFormat="1">
+    <row r="5" spans="1:28" s="65" customFormat="1">
       <c r="A5" s="18" t="s">
         <v>218</v>
       </c>
       <c r="B5" s="20">
         <v>6925</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="81">
         <v>45931</v>
       </c>
       <c r="D5" s="18" t="str">
@@ -9264,7 +9258,7 @@
       <c r="B6" s="18">
         <v>6915</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="81">
         <v>45936</v>
       </c>
       <c r="D6" s="18" t="str">
@@ -9297,7 +9291,7 @@
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
-      <c r="O6" s="55"/>
+      <c r="O6" s="51"/>
       <c r="AA6" s="8" t="s">
         <v>33</v>
       </c>
@@ -9312,7 +9306,7 @@
       <c r="B7" s="18">
         <v>6917</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="81">
         <v>45936</v>
       </c>
       <c r="D7" s="18" t="str">
@@ -9360,7 +9354,7 @@
       <c r="B8" s="18">
         <v>6926</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="81">
         <v>45937</v>
       </c>
       <c r="D8" s="18">
@@ -9407,7 +9401,7 @@
       <c r="B9" s="18">
         <v>6927</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="81">
         <v>45937</v>
       </c>
       <c r="D9" s="18">
@@ -9456,7 +9450,7 @@
       <c r="B10" s="18">
         <v>6916</v>
       </c>
-      <c r="C10" s="45">
+      <c r="C10" s="81">
         <v>45937</v>
       </c>
       <c r="D10" s="18">
@@ -9498,7 +9492,7 @@
       <c r="B11" s="18">
         <v>6911</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C11" s="81">
         <v>45937</v>
       </c>
       <c r="D11" s="18">
@@ -9540,7 +9534,7 @@
       <c r="B12" s="18">
         <v>6912</v>
       </c>
-      <c r="C12" s="45">
+      <c r="C12" s="81">
         <v>45937</v>
       </c>
       <c r="D12" s="18">
@@ -9581,7 +9575,7 @@
       <c r="B13" s="18">
         <v>6908</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="81">
         <v>45937</v>
       </c>
       <c r="D13" s="18">
@@ -9622,7 +9616,7 @@
       <c r="B14" s="18">
         <v>6913</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C14" s="81">
         <v>45937</v>
       </c>
       <c r="D14" s="18">
@@ -9665,7 +9659,7 @@
       <c r="B15" s="18">
         <v>6914</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="81">
         <v>45937</v>
       </c>
       <c r="D15" s="18">
@@ -9704,10 +9698,10 @@
       <c r="A16" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="46">
         <v>7044</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="81">
         <v>45937</v>
       </c>
       <c r="D16" s="18">
@@ -9764,7 +9758,7 @@
       <c r="B17" s="18">
         <v>6943</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="81">
         <v>45937</v>
       </c>
       <c r="D17" s="18">
@@ -9805,7 +9799,7 @@
       <c r="B18" s="18">
         <v>6894</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="81">
         <v>45942</v>
       </c>
       <c r="D18" s="18">
@@ -9849,7 +9843,7 @@
       <c r="B19" s="18">
         <v>6896</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="81">
         <v>45942</v>
       </c>
       <c r="D19" s="18">
@@ -9893,7 +9887,7 @@
       <c r="B20" s="18">
         <v>6895</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="81">
         <v>45942</v>
       </c>
       <c r="D20" s="18">
@@ -9933,7 +9927,7 @@
         <v>235</v>
       </c>
       <c r="B21" s="17"/>
-      <c r="C21" s="45">
+      <c r="C21" s="81">
         <v>45943</v>
       </c>
       <c r="D21" s="18">
@@ -9988,7 +9982,7 @@
       <c r="B22" s="18">
         <v>6886</v>
       </c>
-      <c r="C22" s="45">
+      <c r="C22" s="81">
         <v>45944</v>
       </c>
       <c r="D22" s="18">
@@ -10028,7 +10022,7 @@
         <v>237</v>
       </c>
       <c r="B23" s="18"/>
-      <c r="C23" s="45">
+      <c r="C23" s="81">
         <v>45944</v>
       </c>
       <c r="D23" s="18">
@@ -10072,7 +10066,7 @@
       <c r="B24" s="18">
         <v>6933</v>
       </c>
-      <c r="C24" s="45">
+      <c r="C24" s="81">
         <v>45944</v>
       </c>
       <c r="D24" s="18">
@@ -10114,7 +10108,7 @@
       <c r="B25" s="18">
         <v>7010</v>
       </c>
-      <c r="C25" s="45">
+      <c r="C25" s="81">
         <v>45944</v>
       </c>
       <c r="D25" s="18">
@@ -10156,7 +10150,7 @@
       <c r="B26" s="18">
         <v>6790</v>
       </c>
-      <c r="C26" s="45">
+      <c r="C26" s="81">
         <v>45944</v>
       </c>
       <c r="D26" s="18">
@@ -10198,7 +10192,7 @@
       <c r="B27" s="18">
         <v>6899</v>
       </c>
-      <c r="C27" s="45">
+      <c r="C27" s="81">
         <v>45944</v>
       </c>
       <c r="D27" s="18">
@@ -10242,7 +10236,7 @@
       <c r="B28" s="18">
         <v>6828</v>
       </c>
-      <c r="C28" s="45">
+      <c r="C28" s="81">
         <v>45944</v>
       </c>
       <c r="D28" s="18">
@@ -10284,7 +10278,7 @@
       <c r="B29" s="38">
         <v>5811</v>
       </c>
-      <c r="C29" s="59">
+      <c r="C29" s="82">
         <v>45944</v>
       </c>
       <c r="D29" s="18">
@@ -10321,10 +10315,10 @@
       <c r="A30" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="B30" s="48">
+      <c r="B30" s="46">
         <v>7073</v>
       </c>
-      <c r="C30" s="45">
+      <c r="C30" s="81">
         <v>45944</v>
       </c>
       <c r="D30" s="18">
@@ -10361,8 +10355,8 @@
       <c r="A31" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="B31" s="84"/>
-      <c r="C31" s="45">
+      <c r="B31" s="79"/>
+      <c r="C31" s="81">
         <v>45945</v>
       </c>
       <c r="D31" s="18">
@@ -10390,11 +10384,11 @@
       <c r="O31" s="18"/>
     </row>
     <row r="32" spans="1:28">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="52" t="s">
         <v>246</v>
       </c>
-      <c r="B32" s="56"/>
-      <c r="C32" s="45">
+      <c r="B32" s="52"/>
+      <c r="C32" s="81">
         <v>45951</v>
       </c>
       <c r="D32" s="18">
@@ -10428,13 +10422,13 @@
       <c r="O32" s="18"/>
     </row>
     <row r="33" spans="1:28">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="44" t="s">
         <v>247</v>
       </c>
       <c r="B33" s="18">
         <v>6988</v>
       </c>
-      <c r="C33" s="45">
+      <c r="C33" s="81">
         <v>45951</v>
       </c>
       <c r="D33" s="18">
@@ -10477,7 +10471,7 @@
       <c r="B34" s="18">
         <v>6940</v>
       </c>
-      <c r="C34" s="45">
+      <c r="C34" s="81">
         <v>45951</v>
       </c>
       <c r="D34" s="18">
@@ -10519,7 +10513,7 @@
       <c r="B35" s="18">
         <v>6939</v>
       </c>
-      <c r="C35" s="45">
+      <c r="C35" s="81">
         <v>45951</v>
       </c>
       <c r="D35" s="18">
@@ -10563,7 +10557,7 @@
       <c r="B36" s="18">
         <v>6942</v>
       </c>
-      <c r="C36" s="45">
+      <c r="C36" s="81">
         <v>45951</v>
       </c>
       <c r="D36" s="18">
@@ -10607,7 +10601,7 @@
       <c r="B37" s="18">
         <v>6994</v>
       </c>
-      <c r="C37" s="45">
+      <c r="C37" s="81">
         <v>45951</v>
       </c>
       <c r="D37" s="18">
@@ -10649,7 +10643,7 @@
       <c r="B38" s="18">
         <v>6938</v>
       </c>
-      <c r="C38" s="45">
+      <c r="C38" s="81">
         <v>45951</v>
       </c>
       <c r="D38" s="18">
@@ -10691,7 +10685,7 @@
       <c r="B39" s="18">
         <v>6937</v>
       </c>
-      <c r="C39" s="45">
+      <c r="C39" s="81">
         <v>45951</v>
       </c>
       <c r="D39" s="18">
@@ -10733,7 +10727,7 @@
       <c r="B40" s="18">
         <v>6720</v>
       </c>
-      <c r="C40" s="45">
+      <c r="C40" s="81">
         <v>45956</v>
       </c>
       <c r="D40" s="18">
@@ -10775,7 +10769,7 @@
       <c r="B41" s="18">
         <v>6722</v>
       </c>
-      <c r="C41" s="45">
+      <c r="C41" s="81">
         <v>45956</v>
       </c>
       <c r="D41" s="18">
@@ -10817,7 +10811,7 @@
       <c r="B42" s="38">
         <v>6997</v>
       </c>
-      <c r="C42" s="45">
+      <c r="C42" s="81">
         <v>45957</v>
       </c>
       <c r="D42" s="18">
@@ -10861,7 +10855,7 @@
       <c r="B43" s="18">
         <v>6996</v>
       </c>
-      <c r="C43" s="45">
+      <c r="C43" s="81">
         <v>45958</v>
       </c>
       <c r="D43" s="18">
@@ -10904,7 +10898,7 @@
       <c r="B44" s="18">
         <v>6974</v>
       </c>
-      <c r="C44" s="45">
+      <c r="C44" s="81">
         <v>45958</v>
       </c>
       <c r="D44" s="18">
@@ -10946,7 +10940,7 @@
       <c r="B45" s="18">
         <v>6746</v>
       </c>
-      <c r="C45" s="45">
+      <c r="C45" s="81">
         <v>45958</v>
       </c>
       <c r="D45" s="18">
@@ -10987,7 +10981,7 @@
       <c r="B46" s="18">
         <v>7040</v>
       </c>
-      <c r="C46" s="45">
+      <c r="C46" s="81">
         <v>45958</v>
       </c>
       <c r="D46" s="18">
@@ -11029,7 +11023,7 @@
       <c r="B47" s="18">
         <v>6976</v>
       </c>
-      <c r="C47" s="45">
+      <c r="C47" s="81">
         <v>45958</v>
       </c>
       <c r="D47" s="18">
@@ -11069,7 +11063,7 @@
         <v>264</v>
       </c>
       <c r="B48" s="18"/>
-      <c r="C48" s="45">
+      <c r="C48" s="81">
         <v>45958</v>
       </c>
       <c r="D48" s="18">
@@ -11111,7 +11105,7 @@
         <v>265</v>
       </c>
       <c r="B49" s="18"/>
-      <c r="C49" s="45">
+      <c r="C49" s="81">
         <v>45958</v>
       </c>
       <c r="D49" s="18">
@@ -11151,7 +11145,7 @@
         <v>266</v>
       </c>
       <c r="B50" s="18"/>
-      <c r="C50" s="45">
+      <c r="C50" s="81">
         <v>45958</v>
       </c>
       <c r="D50" s="18">
@@ -11195,7 +11189,7 @@
       <c r="B51" s="18">
         <v>6973</v>
       </c>
-      <c r="C51" s="45">
+      <c r="C51" s="81">
         <v>45958</v>
       </c>
       <c r="D51" s="18">
@@ -11237,7 +11231,7 @@
       <c r="B52" s="18">
         <v>6961</v>
       </c>
-      <c r="C52" s="45">
+      <c r="C52" s="81">
         <v>45958</v>
       </c>
       <c r="D52" s="18">
@@ -11279,7 +11273,7 @@
       <c r="B53" s="18">
         <v>6962</v>
       </c>
-      <c r="C53" s="45">
+      <c r="C53" s="81">
         <v>45958</v>
       </c>
       <c r="D53" s="18">
@@ -11318,10 +11312,10 @@
       <c r="A54" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="B54" s="47">
+      <c r="B54" s="45">
         <v>6978</v>
       </c>
-      <c r="C54" s="45">
+      <c r="C54" s="81">
         <v>45958</v>
       </c>
       <c r="D54" s="18">
@@ -11360,10 +11354,10 @@
       <c r="A55" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="B55" s="47">
+      <c r="B55" s="45">
         <v>6975</v>
       </c>
-      <c r="C55" s="45">
+      <c r="C55" s="81">
         <v>45958</v>
       </c>
       <c r="D55" s="18">
@@ -11405,7 +11399,7 @@
       <c r="B56" s="18">
         <v>6981</v>
       </c>
-      <c r="C56" s="45">
+      <c r="C56" s="81">
         <v>45958</v>
       </c>
       <c r="D56" s="18">
@@ -11446,10 +11440,10 @@
       <c r="A57" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="B57" s="47">
+      <c r="B57" s="45">
         <v>6960</v>
       </c>
-      <c r="C57" s="45">
+      <c r="C57" s="81">
         <v>45958</v>
       </c>
       <c r="D57" s="18">
@@ -11490,10 +11484,10 @@
       <c r="A58" s="31" t="s">
         <v>276</v>
       </c>
-      <c r="B58" s="82">
+      <c r="B58" s="77">
         <v>6977</v>
       </c>
-      <c r="C58" s="59">
+      <c r="C58" s="82">
         <v>45958</v>
       </c>
       <c r="D58" s="31">
@@ -11532,7 +11526,7 @@
       <c r="A59" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="C59" s="45">
+      <c r="C59" s="81">
         <v>45958</v>
       </c>
       <c r="D59" s="18">
@@ -11574,15 +11568,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911F480B-29A9-455F-A268-68331B0D089C}">
   <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="45.5" style="37" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.625" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.25" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.25" style="34" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.625" style="34" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.25" style="34" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.25" style="34" customWidth="1"/>
@@ -11635,13 +11629,13 @@
       <c r="K1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="77" t="s">
+      <c r="L1" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="76" t="s">
+      <c r="M1" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="76" t="s">
+      <c r="N1" s="71" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="41" t="s">
@@ -11655,7 +11649,7 @@
       <c r="B2" s="39">
         <v>6985</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="80">
         <v>45965</v>
       </c>
       <c r="D2" s="43">
@@ -11685,7 +11679,7 @@
       <c r="K2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="78"/>
+      <c r="L2" s="73"/>
       <c r="M2" s="19"/>
       <c r="N2" s="19"/>
       <c r="O2" s="19"/>
@@ -11697,7 +11691,7 @@
       <c r="B3" s="39">
         <v>7060</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="80">
         <v>45965</v>
       </c>
       <c r="D3" s="43">
@@ -11727,7 +11721,7 @@
       <c r="K3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="78"/>
+      <c r="L3" s="73"/>
       <c r="M3" s="19"/>
       <c r="N3" s="19"/>
       <c r="O3" s="19"/>
@@ -11739,7 +11733,7 @@
       <c r="B4" s="39">
         <v>6993</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="80">
         <v>45965</v>
       </c>
       <c r="D4" s="43">
@@ -11769,7 +11763,7 @@
       <c r="K4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="78"/>
+      <c r="L4" s="73"/>
       <c r="M4" s="19"/>
       <c r="N4" s="19"/>
       <c r="O4" s="19"/>
@@ -11781,7 +11775,7 @@
       <c r="B5" s="39">
         <v>6984</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="80">
         <v>45965</v>
       </c>
       <c r="D5" s="43">
@@ -11811,7 +11805,7 @@
       <c r="K5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="78"/>
+      <c r="L5" s="73"/>
       <c r="M5" s="19"/>
       <c r="N5" s="19"/>
       <c r="O5" s="19"/>
@@ -11823,7 +11817,7 @@
       <c r="B6" s="39">
         <v>6986</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="80">
         <v>45965</v>
       </c>
       <c r="D6" s="43">
@@ -11853,7 +11847,7 @@
       <c r="K6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="78"/>
+      <c r="L6" s="73"/>
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
@@ -11869,7 +11863,7 @@
         <v>284</v>
       </c>
       <c r="B7" s="39"/>
-      <c r="C7" s="44">
+      <c r="C7" s="80">
         <v>45965</v>
       </c>
       <c r="D7" s="43">
@@ -11899,7 +11893,7 @@
       <c r="K7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="79"/>
+      <c r="L7" s="74"/>
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
       <c r="O7" s="19"/>
@@ -11917,7 +11911,7 @@
       <c r="B8" s="39">
         <v>6987</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="80">
         <v>45965</v>
       </c>
       <c r="D8" s="43">
@@ -11947,7 +11941,7 @@
       <c r="K8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="78"/>
+      <c r="L8" s="73"/>
       <c r="M8" s="19"/>
       <c r="N8" s="19"/>
       <c r="O8" s="19"/>
@@ -11965,7 +11959,7 @@
       <c r="B9" s="39">
         <v>6983</v>
       </c>
-      <c r="C9" s="44">
+      <c r="C9" s="80">
         <v>45965</v>
       </c>
       <c r="D9" s="43">
@@ -11995,7 +11989,7 @@
       <c r="K9" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="78" t="s">
+      <c r="L9" s="73" t="s">
         <v>287</v>
       </c>
       <c r="M9" s="19"/>
@@ -12015,7 +12009,7 @@
       <c r="B10" s="39">
         <v>6929</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="80">
         <v>45965</v>
       </c>
       <c r="D10" s="43">
@@ -12045,7 +12039,7 @@
       <c r="K10" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="78"/>
+      <c r="L10" s="73"/>
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
@@ -12063,7 +12057,7 @@
       <c r="B11" s="39">
         <v>6857</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="80">
         <v>45965</v>
       </c>
       <c r="D11" s="43">
@@ -12093,7 +12087,7 @@
       <c r="K11" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="78"/>
+      <c r="L11" s="73"/>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
@@ -12105,7 +12099,7 @@
       <c r="B12" s="39">
         <v>7059</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="80">
         <v>45965</v>
       </c>
       <c r="D12" s="43">
@@ -12135,7 +12129,7 @@
       <c r="K12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="78"/>
+      <c r="L12" s="73"/>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
       <c r="O12" s="19"/>
@@ -12147,7 +12141,7 @@
       <c r="B13" s="39">
         <v>7066</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="80">
         <v>45965</v>
       </c>
       <c r="D13" s="43">
@@ -12177,7 +12171,7 @@
       <c r="K13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="78"/>
+      <c r="L13" s="73"/>
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>
@@ -12189,7 +12183,7 @@
       <c r="B14" s="39">
         <v>7064</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="80">
         <v>45965</v>
       </c>
       <c r="D14" s="43">
@@ -12219,7 +12213,7 @@
       <c r="K14" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="78"/>
+      <c r="L14" s="73"/>
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
       <c r="O14" s="19"/>
@@ -12229,7 +12223,7 @@
         <v>293</v>
       </c>
       <c r="B15" s="39"/>
-      <c r="C15" s="44">
+      <c r="C15" s="80">
         <v>45971</v>
       </c>
       <c r="D15" s="43">
@@ -12258,7 +12252,7 @@
       <c r="K15" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L15" s="78"/>
+      <c r="L15" s="73"/>
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
       <c r="O15" s="19"/>
@@ -12268,7 +12262,7 @@
         <v>294</v>
       </c>
       <c r="B16" s="39"/>
-      <c r="C16" s="44">
+      <c r="C16" s="80">
         <v>45971</v>
       </c>
       <c r="D16" s="43">
@@ -12297,7 +12291,7 @@
       <c r="K16" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L16" s="78"/>
+      <c r="L16" s="73"/>
       <c r="M16" s="19"/>
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
@@ -12307,7 +12301,7 @@
         <v>295</v>
       </c>
       <c r="B17" s="39"/>
-      <c r="C17" s="44">
+      <c r="C17" s="80">
         <v>45971</v>
       </c>
       <c r="D17" s="43">
@@ -12336,7 +12330,7 @@
       <c r="K17" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L17" s="78"/>
+      <c r="L17" s="73"/>
       <c r="M17" s="19"/>
       <c r="N17" s="19"/>
       <c r="O17" s="19"/>
@@ -12346,7 +12340,7 @@
         <v>296</v>
       </c>
       <c r="B18" s="39"/>
-      <c r="C18" s="44">
+      <c r="C18" s="80">
         <v>45971</v>
       </c>
       <c r="D18" s="43">
@@ -12375,7 +12369,7 @@
       <c r="K18" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L18" s="78"/>
+      <c r="L18" s="73"/>
       <c r="M18" s="19"/>
       <c r="N18" s="19"/>
       <c r="O18" s="19"/>
@@ -12385,7 +12379,7 @@
         <v>297</v>
       </c>
       <c r="B19" s="39"/>
-      <c r="C19" s="44">
+      <c r="C19" s="80">
         <v>45971</v>
       </c>
       <c r="D19" s="43">
@@ -12414,7 +12408,7 @@
       <c r="K19" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L19" s="78"/>
+      <c r="L19" s="73"/>
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
       <c r="O19" s="19"/>
@@ -12426,7 +12420,7 @@
       <c r="B20" s="39">
         <v>7005</v>
       </c>
-      <c r="C20" s="44">
+      <c r="C20" s="80">
         <v>45972</v>
       </c>
       <c r="D20" s="43">
@@ -12456,7 +12450,7 @@
       <c r="K20" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L20" s="78"/>
+      <c r="L20" s="73"/>
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
       <c r="O20" s="19"/>
@@ -12468,7 +12462,7 @@
       <c r="B21" s="39">
         <v>7054</v>
       </c>
-      <c r="C21" s="44">
+      <c r="C21" s="80">
         <v>45972</v>
       </c>
       <c r="D21" s="43">
@@ -12498,7 +12492,7 @@
       <c r="K21" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L21" s="78" t="s">
+      <c r="L21" s="73" t="s">
         <v>287</v>
       </c>
       <c r="M21" s="19"/>
@@ -12512,7 +12506,7 @@
       <c r="B22" s="39">
         <v>6991</v>
       </c>
-      <c r="C22" s="44">
+      <c r="C22" s="80">
         <v>45972</v>
       </c>
       <c r="D22" s="43">
@@ -12542,7 +12536,7 @@
       <c r="K22" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L22" s="78"/>
+      <c r="L22" s="73"/>
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
       <c r="O22" s="19"/>
@@ -12554,7 +12548,7 @@
       <c r="B23" s="39">
         <v>6990</v>
       </c>
-      <c r="C23" s="44">
+      <c r="C23" s="80">
         <v>45972</v>
       </c>
       <c r="D23" s="43">
@@ -12584,7 +12578,7 @@
       <c r="K23" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="78"/>
+      <c r="L23" s="73"/>
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
       <c r="O23" s="19"/>
@@ -12596,7 +12590,7 @@
       <c r="B24" s="39">
         <v>6992</v>
       </c>
-      <c r="C24" s="44">
+      <c r="C24" s="80">
         <v>45972</v>
       </c>
       <c r="D24" s="43">
@@ -12626,7 +12620,7 @@
       <c r="K24" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L24" s="78"/>
+      <c r="L24" s="73"/>
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
       <c r="O24" s="19"/>
@@ -12638,7 +12632,7 @@
       <c r="B25" s="39">
         <v>6922</v>
       </c>
-      <c r="C25" s="44">
+      <c r="C25" s="80">
         <v>45972</v>
       </c>
       <c r="D25" s="43">
@@ -12665,7 +12659,7 @@
       <c r="K25" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L25" s="78"/>
+      <c r="L25" s="73"/>
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
       <c r="O25" s="19"/>
@@ -12675,7 +12669,7 @@
         <v>304</v>
       </c>
       <c r="B26" s="39"/>
-      <c r="C26" s="44">
+      <c r="C26" s="80">
         <v>45972</v>
       </c>
       <c r="D26" s="43">
@@ -12705,7 +12699,7 @@
       <c r="K26" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L26" s="78"/>
+      <c r="L26" s="73"/>
       <c r="M26" s="19"/>
       <c r="N26" s="19"/>
       <c r="O26" s="19"/>
@@ -12715,7 +12709,7 @@
         <v>305</v>
       </c>
       <c r="B27" s="39"/>
-      <c r="C27" s="44">
+      <c r="C27" s="80">
         <v>45972</v>
       </c>
       <c r="D27" s="43">
@@ -12745,7 +12739,7 @@
       <c r="K27" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L27" s="78" t="s">
+      <c r="L27" s="73" t="s">
         <v>306</v>
       </c>
       <c r="M27" s="19"/>
@@ -12759,14 +12753,14 @@
       <c r="B28" s="39">
         <v>2262</v>
       </c>
-      <c r="C28" s="44">
+      <c r="C28" s="80">
         <v>45972</v>
       </c>
       <c r="D28" s="43">
         <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="50" t="s">
         <v>85</v>
       </c>
       <c r="F28" s="39" t="str">
@@ -12789,7 +12783,7 @@
       <c r="K28" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L28" s="78"/>
+      <c r="L28" s="73"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
       <c r="O28" s="19"/>
@@ -12801,7 +12795,7 @@
       <c r="B29" s="39">
         <v>7032</v>
       </c>
-      <c r="C29" s="44">
+      <c r="C29" s="80">
         <v>45972</v>
       </c>
       <c r="D29" s="43">
@@ -12831,7 +12825,7 @@
       <c r="K29" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L29" s="78"/>
+      <c r="L29" s="73"/>
       <c r="M29" s="19"/>
       <c r="N29" s="19"/>
       <c r="O29" s="19"/>
@@ -12843,7 +12837,7 @@
       <c r="B30" s="39">
         <v>6964</v>
       </c>
-      <c r="C30" s="44">
+      <c r="C30" s="80">
         <v>45972</v>
       </c>
       <c r="D30" s="43">
@@ -12873,7 +12867,7 @@
       <c r="K30" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L30" s="78"/>
+      <c r="L30" s="73"/>
       <c r="M30" s="19"/>
       <c r="N30" s="19"/>
       <c r="O30" s="19"/>
@@ -12885,7 +12879,7 @@
       <c r="B31" s="39">
         <v>7004</v>
       </c>
-      <c r="C31" s="44">
+      <c r="C31" s="80">
         <v>45972</v>
       </c>
       <c r="D31" s="43">
@@ -12915,7 +12909,7 @@
       <c r="K31" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L31" s="78"/>
+      <c r="L31" s="73"/>
       <c r="M31" s="19"/>
       <c r="N31" s="19"/>
       <c r="O31" s="19"/>
@@ -12924,10 +12918,10 @@
       <c r="A32" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="B32" s="50">
+      <c r="B32" s="48">
         <v>6924</v>
       </c>
-      <c r="C32" s="44">
+      <c r="C32" s="80">
         <v>45972</v>
       </c>
       <c r="D32" s="43">
@@ -12956,7 +12950,7 @@
       <c r="K32" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L32" s="78"/>
+      <c r="L32" s="73"/>
       <c r="M32" s="19"/>
       <c r="N32" s="19"/>
       <c r="O32" s="19"/>
@@ -12968,7 +12962,7 @@
       <c r="B33" s="39">
         <v>7043</v>
       </c>
-      <c r="C33" s="44">
+      <c r="C33" s="80">
         <v>45972</v>
       </c>
       <c r="D33" s="43">
@@ -12998,7 +12992,7 @@
       <c r="K33" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L33" s="78"/>
+      <c r="L33" s="73"/>
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
       <c r="O33" s="19"/>
@@ -13010,7 +13004,7 @@
       <c r="B34" s="39">
         <v>6930</v>
       </c>
-      <c r="C34" s="44">
+      <c r="C34" s="80">
         <v>45972</v>
       </c>
       <c r="D34" s="43">
@@ -13040,7 +13034,7 @@
       <c r="K34" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L34" s="78"/>
+      <c r="L34" s="73"/>
       <c r="M34" s="19"/>
       <c r="N34" s="19"/>
       <c r="O34" s="19"/>
@@ -13052,7 +13046,7 @@
       <c r="B35" s="39">
         <v>7036</v>
       </c>
-      <c r="C35" s="44">
+      <c r="C35" s="80">
         <v>45972</v>
       </c>
       <c r="D35" s="43">
@@ -13082,7 +13076,7 @@
       <c r="K35" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L35" s="78"/>
+      <c r="L35" s="73"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
@@ -13094,7 +13088,7 @@
       <c r="B36" s="39">
         <v>7034</v>
       </c>
-      <c r="C36" s="44">
+      <c r="C36" s="80">
         <v>45972</v>
       </c>
       <c r="D36" s="43">
@@ -13124,7 +13118,7 @@
       <c r="K36" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L36" s="78"/>
+      <c r="L36" s="73"/>
       <c r="M36" s="19"/>
       <c r="N36" s="19"/>
       <c r="O36" s="19"/>
@@ -13136,7 +13130,7 @@
       <c r="B37" s="39">
         <v>7035</v>
       </c>
-      <c r="C37" s="44">
+      <c r="C37" s="80">
         <v>45972</v>
       </c>
       <c r="D37" s="43">
@@ -13166,7 +13160,7 @@
       <c r="K37" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L37" s="78"/>
+      <c r="L37" s="73"/>
       <c r="M37" s="19"/>
       <c r="N37" s="19"/>
       <c r="O37" s="19"/>
@@ -13178,7 +13172,7 @@
       <c r="B38" s="39">
         <v>7033</v>
       </c>
-      <c r="C38" s="44">
+      <c r="C38" s="80">
         <v>45972</v>
       </c>
       <c r="D38" s="43">
@@ -13208,7 +13202,7 @@
       <c r="K38" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L38" s="78"/>
+      <c r="L38" s="73"/>
       <c r="M38" s="19"/>
       <c r="N38" s="19"/>
       <c r="O38" s="19"/>
@@ -13220,7 +13214,7 @@
       <c r="B39" s="39">
         <v>6668</v>
       </c>
-      <c r="C39" s="44">
+      <c r="C39" s="80">
         <v>45977</v>
       </c>
       <c r="D39" s="43">
@@ -13250,7 +13244,7 @@
       <c r="K39" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L39" s="78"/>
+      <c r="L39" s="73"/>
       <c r="M39" s="19"/>
       <c r="N39" s="19"/>
       <c r="O39" s="19"/>
@@ -13262,7 +13256,7 @@
       <c r="B40" s="39">
         <v>6972</v>
       </c>
-      <c r="C40" s="44">
+      <c r="C40" s="80">
         <v>45979</v>
       </c>
       <c r="D40" s="43">
@@ -13292,7 +13286,7 @@
       <c r="K40" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L40" s="78"/>
+      <c r="L40" s="73"/>
       <c r="M40" s="19"/>
       <c r="N40" s="19"/>
       <c r="O40" s="19"/>
@@ -13304,7 +13298,7 @@
       <c r="B41" s="39">
         <v>7025</v>
       </c>
-      <c r="C41" s="44">
+      <c r="C41" s="80">
         <v>45979</v>
       </c>
       <c r="D41" s="43">
@@ -13347,7 +13341,7 @@
       <c r="B42" s="39">
         <v>7021</v>
       </c>
-      <c r="C42" s="44">
+      <c r="C42" s="80">
         <v>45979</v>
       </c>
       <c r="D42" s="43">
@@ -13377,7 +13371,7 @@
       <c r="K42" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L42" s="78"/>
+      <c r="L42" s="73"/>
       <c r="M42" s="19"/>
       <c r="N42" s="19"/>
       <c r="O42" s="19"/>
@@ -13389,7 +13383,7 @@
       <c r="B43" s="39">
         <v>7027</v>
       </c>
-      <c r="C43" s="44">
+      <c r="C43" s="80">
         <v>45979</v>
       </c>
       <c r="D43" s="43">
@@ -13419,7 +13413,7 @@
       <c r="K43" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L43" s="78"/>
+      <c r="L43" s="73"/>
       <c r="M43" s="19"/>
       <c r="N43" s="19"/>
       <c r="O43" s="19"/>
@@ -13431,7 +13425,7 @@
       <c r="B44" s="39">
         <v>7026</v>
       </c>
-      <c r="C44" s="44">
+      <c r="C44" s="80">
         <v>45979</v>
       </c>
       <c r="D44" s="43">
@@ -13461,7 +13455,7 @@
       <c r="K44" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L44" s="78"/>
+      <c r="L44" s="73"/>
       <c r="M44" s="19"/>
       <c r="N44" s="19"/>
       <c r="O44" s="19"/>
@@ -13473,7 +13467,7 @@
       <c r="B45" s="39">
         <v>7024</v>
       </c>
-      <c r="C45" s="44">
+      <c r="C45" s="80">
         <v>45979</v>
       </c>
       <c r="D45" s="43">
@@ -13500,10 +13494,10 @@
       <c r="J45" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="K45" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="L45" s="78"/>
+      <c r="K45" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="L45" s="73"/>
       <c r="M45" s="19"/>
       <c r="N45" s="19"/>
       <c r="O45" s="19"/>
@@ -13515,7 +13509,7 @@
       <c r="B46" s="39">
         <v>7022</v>
       </c>
-      <c r="C46" s="44">
+      <c r="C46" s="80">
         <v>45979</v>
       </c>
       <c r="D46" s="43">
@@ -13545,7 +13539,7 @@
       <c r="K46" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L46" s="78"/>
+      <c r="L46" s="73"/>
       <c r="M46" s="19"/>
       <c r="N46" s="19"/>
       <c r="O46" s="19"/>
@@ -13557,7 +13551,7 @@
       <c r="B47" s="39">
         <v>7023</v>
       </c>
-      <c r="C47" s="44">
+      <c r="C47" s="80">
         <v>45979</v>
       </c>
       <c r="D47" s="43">
@@ -13587,7 +13581,7 @@
       <c r="K47" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L47" s="78"/>
+      <c r="L47" s="73"/>
       <c r="M47" s="19"/>
       <c r="N47" s="19"/>
       <c r="O47" s="19"/>
@@ -13599,7 +13593,7 @@
       <c r="B48" s="39">
         <v>6963</v>
       </c>
-      <c r="C48" s="44">
+      <c r="C48" s="80">
         <v>45979</v>
       </c>
       <c r="D48" s="43">
@@ -13629,7 +13623,7 @@
       <c r="K48" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="L48" s="78"/>
+      <c r="L48" s="73"/>
       <c r="M48" s="19"/>
       <c r="N48" s="19"/>
       <c r="O48" s="19"/>
@@ -13641,7 +13635,7 @@
       <c r="B49" s="39">
         <v>7019</v>
       </c>
-      <c r="C49" s="44">
+      <c r="C49" s="80">
         <v>45979</v>
       </c>
       <c r="D49" s="43">
@@ -13668,39 +13662,39 @@
       <c r="J49" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="K49" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="L49" s="78"/>
+      <c r="K49" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="L49" s="73"/>
       <c r="M49" s="19"/>
       <c r="N49" s="19"/>
       <c r="O49" s="19"/>
     </row>
     <row r="50" spans="1:16">
-      <c r="A50" s="51" t="s">
+      <c r="A50" s="49" t="s">
         <v>329</v>
       </c>
-      <c r="B50" s="51">
+      <c r="B50" s="49">
         <v>7017</v>
       </c>
-      <c r="C50" s="52">
+      <c r="C50" s="80">
         <v>45979</v>
       </c>
       <c r="D50" s="43">
         <f t="shared" ca="1" si="0"/>
         <v>42</v>
       </c>
-      <c r="E50" s="51" t="s">
+      <c r="E50" s="49" t="s">
         <v>83</v>
       </c>
       <c r="F50" s="39" t="str">
         <f>VLOOKUP(E50,'October Go Live'!E:F,2,0)</f>
         <v>Angie Bogart</v>
       </c>
-      <c r="G50" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="H50" s="51" t="s">
+      <c r="G50" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="H50" s="49" t="s">
         <v>33</v>
       </c>
       <c r="I50" s="28" t="str">
@@ -13713,7 +13707,7 @@
       <c r="K50" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="L50" s="80"/>
+      <c r="L50" s="75"/>
       <c r="M50" s="19"/>
       <c r="N50" s="19"/>
       <c r="O50" s="19"/>
@@ -13725,7 +13719,7 @@
       <c r="B51" s="19">
         <v>6989</v>
       </c>
-      <c r="C51" s="44">
+      <c r="C51" s="80">
         <v>45979</v>
       </c>
       <c r="D51" s="43">
@@ -13754,8 +13748,8 @@
       <c r="K51" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L51" s="78"/>
-      <c r="P51" s="81"/>
+      <c r="L51" s="73"/>
+      <c r="P51" s="76"/>
     </row>
     <row r="52" spans="1:16">
       <c r="A52" s="19" t="s">
@@ -13764,7 +13758,7 @@
       <c r="B52" s="19">
         <v>7082</v>
       </c>
-      <c r="C52" s="44">
+      <c r="C52" s="80">
         <v>45985</v>
       </c>
       <c r="D52" s="43">
@@ -13836,14 +13830,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D228CD-9D9F-4237-BD9A-B6017414C1EE}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="43.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
@@ -13901,7 +13895,7 @@
       <c r="B2" s="19">
         <v>6770</v>
       </c>
-      <c r="C2" s="53">
+      <c r="C2" s="80">
         <v>45992</v>
       </c>
       <c r="D2" s="43">
@@ -13936,7 +13930,7 @@
         <v>333</v>
       </c>
       <c r="B3" s="19"/>
-      <c r="C3" s="53">
+      <c r="C3" s="80">
         <v>45993</v>
       </c>
       <c r="D3" s="43">
@@ -13971,7 +13965,7 @@
         <v>334</v>
       </c>
       <c r="B4" s="19"/>
-      <c r="C4" s="53">
+      <c r="C4" s="80">
         <v>45993</v>
       </c>
       <c r="D4" s="43">
@@ -14012,7 +14006,7 @@
         <v>335</v>
       </c>
       <c r="B5" s="19"/>
-      <c r="C5" s="53">
+      <c r="C5" s="80">
         <v>45993</v>
       </c>
       <c r="D5" s="43">
@@ -14053,7 +14047,7 @@
         <v>336</v>
       </c>
       <c r="B6" s="19"/>
-      <c r="C6" s="53">
+      <c r="C6" s="80">
         <v>45993</v>
       </c>
       <c r="D6" s="43">
@@ -14095,7 +14089,7 @@
       <c r="B7" s="19">
         <v>7067</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="80">
         <v>45993</v>
       </c>
       <c r="D7" s="43">
@@ -14138,7 +14132,7 @@
       <c r="B8" s="19">
         <v>7069</v>
       </c>
-      <c r="C8" s="53">
+      <c r="C8" s="80">
         <v>45993</v>
       </c>
       <c r="D8" s="43">
@@ -14181,7 +14175,7 @@
       <c r="B9" s="19">
         <v>7068</v>
       </c>
-      <c r="C9" s="53">
+      <c r="C9" s="80">
         <v>45993</v>
       </c>
       <c r="D9" s="43">
@@ -14216,7 +14210,7 @@
         <v>340</v>
       </c>
       <c r="B10" s="19"/>
-      <c r="C10" s="53">
+      <c r="C10" s="80">
         <v>45993</v>
       </c>
       <c r="D10" s="43">
@@ -14252,7 +14246,7 @@
       <c r="B11" s="19">
         <v>7081</v>
       </c>
-      <c r="C11" s="53">
+      <c r="C11" s="80">
         <v>46000</v>
       </c>
       <c r="D11" s="43">
@@ -14287,7 +14281,7 @@
         <v>342</v>
       </c>
       <c r="B12" s="19"/>
-      <c r="C12" s="53">
+      <c r="C12" s="80">
         <v>46000</v>
       </c>
       <c r="D12" s="43">
@@ -14324,7 +14318,7 @@
       <c r="B13" s="19">
         <v>5939</v>
       </c>
-      <c r="C13" s="53">
+      <c r="C13" s="80">
         <v>46000</v>
       </c>
       <c r="D13" s="43">
@@ -14361,7 +14355,7 @@
       <c r="B14" s="19">
         <v>7071</v>
       </c>
-      <c r="C14" s="53">
+      <c r="C14" s="80">
         <v>46000</v>
       </c>
       <c r="D14" s="43">
@@ -14398,7 +14392,7 @@
       <c r="B15" s="19">
         <v>7070</v>
       </c>
-      <c r="C15" s="53">
+      <c r="C15" s="80">
         <v>46000</v>
       </c>
       <c r="D15" s="43">
@@ -14435,7 +14429,7 @@
       <c r="B16" s="19">
         <v>7072</v>
       </c>
-      <c r="C16" s="53">
+      <c r="C16" s="80">
         <v>46000</v>
       </c>
       <c r="D16" s="43">
@@ -14472,7 +14466,7 @@
       <c r="B17" s="19">
         <v>7078</v>
       </c>
-      <c r="C17" s="53">
+      <c r="C17" s="80">
         <v>46000</v>
       </c>
       <c r="D17" s="43">
@@ -14509,7 +14503,7 @@
       <c r="B18" s="19">
         <v>7079</v>
       </c>
-      <c r="C18" s="53">
+      <c r="C18" s="80">
         <v>46000</v>
       </c>
       <c r="D18" s="43">
@@ -14546,7 +14540,7 @@
       <c r="B19" s="19">
         <v>7065</v>
       </c>
-      <c r="C19" s="53">
+      <c r="C19" s="80">
         <v>46000</v>
       </c>
       <c r="D19" s="43">
@@ -14581,7 +14575,7 @@
         <v>350</v>
       </c>
       <c r="B20" s="19"/>
-      <c r="C20" s="53">
+      <c r="C20" s="80">
         <v>46000</v>
       </c>
       <c r="D20" s="43">
@@ -14611,11 +14605,11 @@
       <c r="L20" s="17"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="69" t="s">
         <v>351</v>
       </c>
       <c r="B21" s="19"/>
-      <c r="C21" s="53">
+      <c r="C21" s="80">
         <v>46000</v>
       </c>
       <c r="D21" s="43">
@@ -14649,8 +14643,8 @@
       <c r="A22" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="B22" s="81"/>
-      <c r="C22" s="53">
+      <c r="B22" s="76"/>
+      <c r="C22" s="80">
         <v>46000</v>
       </c>
       <c r="D22" s="43">
@@ -14682,8 +14676,8 @@
       <c r="A23" s="17" t="s">
         <v>353</v>
       </c>
-      <c r="B23" s="81"/>
-      <c r="C23" s="53">
+      <c r="B23" s="76"/>
+      <c r="C23" s="80">
         <v>46000</v>
       </c>
       <c r="D23" s="43">
@@ -14715,8 +14709,8 @@
       <c r="A24" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="53">
+      <c r="B24" s="76"/>
+      <c r="C24" s="80">
         <v>46000</v>
       </c>
       <c r="D24" s="43">
@@ -14748,8 +14742,8 @@
       <c r="A25" s="17" t="s">
         <v>355</v>
       </c>
-      <c r="B25" s="81"/>
-      <c r="C25" s="53">
+      <c r="B25" s="76"/>
+      <c r="C25" s="80">
         <v>46000</v>
       </c>
       <c r="D25" s="43">
@@ -14781,8 +14775,8 @@
       <c r="A26" s="17" t="s">
         <v>356</v>
       </c>
-      <c r="B26" s="81"/>
-      <c r="C26" s="53">
+      <c r="B26" s="76"/>
+      <c r="C26" s="80">
         <v>46000</v>
       </c>
       <c r="D26" s="43">
@@ -14814,8 +14808,8 @@
       <c r="A27" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="B27" s="81"/>
-      <c r="C27" s="53">
+      <c r="B27" s="76"/>
+      <c r="C27" s="80">
         <v>46000</v>
       </c>
       <c r="D27" s="43">
@@ -14845,8 +14839,8 @@
       <c r="A28" s="17" t="s">
         <v>358</v>
       </c>
-      <c r="B28" s="81"/>
-      <c r="C28" s="53">
+      <c r="B28" s="76"/>
+      <c r="C28" s="80">
         <v>46000</v>
       </c>
       <c r="D28" s="43">
@@ -14876,8 +14870,8 @@
       <c r="A29" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="B29" s="81"/>
-      <c r="C29" s="53">
+      <c r="B29" s="76"/>
+      <c r="C29" s="80">
         <v>46000</v>
       </c>
       <c r="D29" s="43">
@@ -14907,8 +14901,8 @@
       <c r="A30" s="17" t="s">
         <v>360</v>
       </c>
-      <c r="B30" s="81"/>
-      <c r="C30" s="53">
+      <c r="B30" s="76"/>
+      <c r="C30" s="80">
         <v>46000</v>
       </c>
       <c r="D30" s="43">
@@ -14939,7 +14933,7 @@
         <v>361</v>
       </c>
       <c r="B31" s="19"/>
-      <c r="C31" s="53">
+      <c r="C31" s="80">
         <v>46000</v>
       </c>
       <c r="D31" s="43">
@@ -14966,11 +14960,11 @@
       <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="69" t="s">
         <v>362</v>
       </c>
       <c r="B32" s="19"/>
-      <c r="C32" s="53">
+      <c r="C32" s="80">
         <v>46006</v>
       </c>
       <c r="D32" s="43">
@@ -15000,8 +14994,8 @@
       <c r="A33" s="17" t="s">
         <v>363</v>
       </c>
-      <c r="B33" s="81"/>
-      <c r="C33" s="53">
+      <c r="B33" s="76"/>
+      <c r="C33" s="80">
         <v>46006</v>
       </c>
       <c r="D33" s="43">
@@ -15025,10 +15019,10 @@
       <c r="A34" s="17" t="s">
         <v>364</v>
       </c>
-      <c r="B34" s="81">
+      <c r="B34" s="76">
         <v>7092</v>
       </c>
-      <c r="C34" s="53">
+      <c r="C34" s="80">
         <v>46006</v>
       </c>
       <c r="D34" s="43">
@@ -15049,11 +15043,11 @@
       <c r="L34" s="17"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="83" t="s">
+      <c r="A35" s="78" t="s">
         <v>365</v>
       </c>
-      <c r="B35" s="81"/>
-      <c r="C35" s="53">
+      <c r="B35" s="76"/>
+      <c r="C35" s="80">
         <v>46006</v>
       </c>
       <c r="D35" s="43">
@@ -15080,11 +15074,11 @@
       <c r="L35" s="17"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="53" t="s">
         <v>366</v>
       </c>
       <c r="B36" s="19"/>
-      <c r="C36" s="53">
+      <c r="C36" s="80">
         <v>46007</v>
       </c>
       <c r="D36" s="43">
@@ -15121,9 +15115,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15271,16 +15268,13 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D4D27E7-ACD2-46B6-AA09-8BF6B6C0F14C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{766BC07B-98D5-4153-A7D7-7129A056142D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15288,5 +15282,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{766BC07B-98D5-4153-A7D7-7129A056142D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D4D27E7-ACD2-46B6-AA09-8BF6B6C0F14C}"/>
 </file>
</xml_diff>